<commit_message>
Changes on Test Cases and Test Stretergy
</commit_message>
<xml_diff>
--- a/loanPredictionTestCase.xlsx
+++ b/loanPredictionTestCase.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -129,16 +129,16 @@
     <t>TC-06</t>
   </si>
   <si>
-    <t>Check Evaluation Metrics</t>
-  </si>
-  <si>
-    <t>Verify that the evaluation details are visible and correct.</t>
-  </si>
-  <si>
-    <t>1. Scroll down to the 'Evaluation' section.</t>
-  </si>
-  <si>
-    <t>Evaluation metrics should be displayed clearly.</t>
+    <t>Check Submit Solution</t>
+  </si>
+  <si>
+    <t>Verify that the Submit Solution Btn visible and redirect to submit solution page.</t>
+  </si>
+  <si>
+    <t>1. Click on Submit Solution Button.</t>
+  </si>
+  <si>
+    <t>Submittion Page will open and there will be add solution Btn.</t>
   </si>
   <si>
     <t>TC-07</t>
@@ -238,17 +238,20 @@
     <t>TC-12</t>
   </si>
   <si>
-    <t>Accessibility Check</t>
-  </si>
-  <si>
-    <t>Run a basic accessibility audit.</t>
-  </si>
-  <si>
-    <t>1. Open Chrome DevTools.
-2. Run Lighthouse accessibility audit.</t>
-  </si>
-  <si>
-    <t>Accessibility score should be at least 70 with no critical issues.</t>
+    <t>Smooth Scrolling and Navigation</t>
+  </si>
+  <si>
+    <t>Verify smooth scrolling and visibility of all sections.</t>
+  </si>
+  <si>
+    <t>1. Scroll slowly through the page.
+2. Check each section for visibility.</t>
+  </si>
+  <si>
+    <t>All sections should load smoothly and be clearly visible.</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
   <si>
     <t>TC-13</t>
@@ -286,25 +289,6 @@
   </si>
   <si>
     <t>Page should load without errors and all sections should work as expected.</t>
-  </si>
-  <si>
-    <t>TC-15</t>
-  </si>
-  <si>
-    <t>Smooth Scrolling and Navigation</t>
-  </si>
-  <si>
-    <t>Verify smooth scrolling and visibility of all sections.</t>
-  </si>
-  <si>
-    <t>1. Scroll slowly through the page.
-2. Check each section for visibility.</t>
-  </si>
-  <si>
-    <t>All sections should load smoothly and be clearly visible.</t>
-  </si>
-  <si>
-    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -766,19 +750,19 @@
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="2"/>
@@ -907,7 +891,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -917,7 +901,7 @@
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>74</v>
@@ -927,27 +911,27 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
@@ -956,52 +940,29 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
+    <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -1981,7 +1942,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>